<commit_message>
Updates to Slides and calculations
</commit_message>
<xml_diff>
--- a/Presentations/Mid Semester Review/Individual_Slides/Tyler/PowerMassBOM3_ABee.xlsx
+++ b/Presentations/Mid Semester Review/Individual_Slides/Tyler/PowerMassBOM3_ABee.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="60" windowWidth="24240" windowHeight="13680" firstSheet="1" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="60" windowWidth="24240" windowHeight="13680" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Battery" sheetId="1" r:id="rId1"/>
@@ -809,69 +809,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -892,6 +829,69 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1208,72 +1208,72 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" s="31" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="96" t="s">
+      <c r="A1" s="104" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="96"/>
-      <c r="C1" s="96"/>
-      <c r="D1" s="96"/>
-      <c r="E1" s="96"/>
-      <c r="F1" s="96"/>
-      <c r="G1" s="96"/>
-      <c r="H1" s="96"/>
-      <c r="I1" s="96"/>
-      <c r="J1" s="96"/>
-      <c r="K1" s="96"/>
-      <c r="L1" s="96"/>
+      <c r="B1" s="104"/>
+      <c r="C1" s="104"/>
+      <c r="D1" s="104"/>
+      <c r="E1" s="104"/>
+      <c r="F1" s="104"/>
+      <c r="G1" s="104"/>
+      <c r="H1" s="104"/>
+      <c r="I1" s="104"/>
+      <c r="J1" s="104"/>
+      <c r="K1" s="104"/>
+      <c r="L1" s="104"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="99" t="s">
+      <c r="A2" s="107" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="97" t="s">
+      <c r="B2" s="105" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="97" t="s">
+      <c r="C2" s="105" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="101" t="s">
+      <c r="D2" s="109" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="103" t="s">
+      <c r="E2" s="111" t="s">
         <v>31</v>
       </c>
-      <c r="F2" s="105" t="s">
+      <c r="F2" s="113" t="s">
         <v>32</v>
       </c>
-      <c r="G2" s="107" t="s">
+      <c r="G2" s="115" t="s">
         <v>33</v>
       </c>
-      <c r="H2" s="105" t="s">
+      <c r="H2" s="113" t="s">
         <v>34</v>
       </c>
-      <c r="I2" s="109" t="s">
+      <c r="I2" s="117" t="s">
         <v>13</v>
       </c>
-      <c r="J2" s="109" t="s">
+      <c r="J2" s="117" t="s">
         <v>14</v>
       </c>
-      <c r="K2" s="109" t="s">
+      <c r="K2" s="117" t="s">
         <v>15</v>
       </c>
-      <c r="L2" s="97" t="s">
+      <c r="L2" s="105" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="100"/>
-      <c r="B3" s="98"/>
-      <c r="C3" s="98"/>
-      <c r="D3" s="102"/>
-      <c r="E3" s="104"/>
-      <c r="F3" s="106"/>
-      <c r="G3" s="108"/>
-      <c r="H3" s="104"/>
-      <c r="I3" s="110"/>
-      <c r="J3" s="110"/>
-      <c r="K3" s="110"/>
-      <c r="L3" s="98"/>
+      <c r="A3" s="108"/>
+      <c r="B3" s="106"/>
+      <c r="C3" s="106"/>
+      <c r="D3" s="110"/>
+      <c r="E3" s="112"/>
+      <c r="F3" s="114"/>
+      <c r="G3" s="116"/>
+      <c r="H3" s="112"/>
+      <c r="I3" s="118"/>
+      <c r="J3" s="118"/>
+      <c r="K3" s="118"/>
+      <c r="L3" s="106"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="36" t="s">
@@ -1366,7 +1366,7 @@
   <dimension ref="A1:N20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1378,60 +1378,60 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" s="31" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="96" t="s">
+      <c r="A1" s="104" t="s">
         <v>36</v>
       </c>
-      <c r="B1" s="96"/>
-      <c r="C1" s="96"/>
-      <c r="D1" s="96"/>
-      <c r="E1" s="96"/>
-      <c r="F1" s="96"/>
-      <c r="G1" s="96"/>
-      <c r="H1" s="96"/>
-      <c r="I1" s="96"/>
-      <c r="J1" s="96"/>
-      <c r="K1" s="96"/>
-      <c r="L1" s="96"/>
-      <c r="M1" s="96"/>
-      <c r="N1" s="96"/>
+      <c r="B1" s="104"/>
+      <c r="C1" s="104"/>
+      <c r="D1" s="104"/>
+      <c r="E1" s="104"/>
+      <c r="F1" s="104"/>
+      <c r="G1" s="104"/>
+      <c r="H1" s="104"/>
+      <c r="I1" s="104"/>
+      <c r="J1" s="104"/>
+      <c r="K1" s="104"/>
+      <c r="L1" s="104"/>
+      <c r="M1" s="104"/>
+      <c r="N1" s="104"/>
     </row>
     <row r="2" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="99" t="s">
+      <c r="A2" s="107" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="97" t="s">
+      <c r="B2" s="105" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="97" t="s">
+      <c r="C2" s="105" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="101" t="s">
+      <c r="D2" s="109" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="111" t="s">
+      <c r="E2" s="119" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="112"/>
-      <c r="G2" s="113"/>
-      <c r="H2" s="111" t="s">
+      <c r="F2" s="120"/>
+      <c r="G2" s="121"/>
+      <c r="H2" s="119" t="s">
         <v>11</v>
       </c>
-      <c r="I2" s="112"/>
-      <c r="J2" s="113"/>
-      <c r="K2" s="111" t="s">
+      <c r="I2" s="120"/>
+      <c r="J2" s="121"/>
+      <c r="K2" s="119" t="s">
         <v>12</v>
       </c>
-      <c r="L2" s="112"/>
-      <c r="M2" s="113"/>
-      <c r="N2" s="97" t="s">
+      <c r="L2" s="120"/>
+      <c r="M2" s="121"/>
+      <c r="N2" s="105" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="100"/>
-      <c r="B3" s="98"/>
-      <c r="C3" s="98"/>
-      <c r="D3" s="102"/>
+      <c r="A3" s="108"/>
+      <c r="B3" s="106"/>
+      <c r="C3" s="106"/>
+      <c r="D3" s="110"/>
       <c r="E3" s="13" t="s">
         <v>17</v>
       </c>
@@ -1459,7 +1459,7 @@
       <c r="M3" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="N3" s="98"/>
+      <c r="N3" s="106"/>
     </row>
     <row r="4" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="76" t="s">
@@ -1490,13 +1490,13 @@
       <c r="J4" s="77">
         <v>13.5</v>
       </c>
-      <c r="K4" s="119">
+      <c r="K4" s="98">
         <v>365.26315789473682</v>
       </c>
-      <c r="L4" s="120">
+      <c r="L4" s="99">
         <v>333.33333333333331</v>
       </c>
-      <c r="M4" s="118">
+      <c r="M4" s="97">
         <v>1040.8333333333333</v>
       </c>
       <c r="N4" s="82" t="s">
@@ -1508,7 +1508,7 @@
         <v>43</v>
       </c>
       <c r="B5" s="77">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C5" s="78">
         <v>64.2</v>
@@ -1524,11 +1524,11 @@
         <v>5</v>
       </c>
       <c r="J5" s="77"/>
-      <c r="K5" s="120"/>
-      <c r="L5" s="120">
+      <c r="K5" s="99"/>
+      <c r="L5" s="99">
         <v>800</v>
       </c>
-      <c r="M5" s="118"/>
+      <c r="M5" s="97"/>
       <c r="N5" s="82" t="s">
         <v>53</v>
       </c>
@@ -1590,7 +1590,7 @@
         <v>25</v>
       </c>
       <c r="K7" s="81"/>
-      <c r="L7" s="117">
+      <c r="L7" s="96">
         <v>540.54054054054052</v>
       </c>
       <c r="M7" s="77"/>
@@ -1601,7 +1601,7 @@
         <v>41</v>
       </c>
       <c r="B8" s="77">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C8" s="78">
         <v>115</v>
@@ -1665,7 +1665,7 @@
         <v>52</v>
       </c>
       <c r="B10" s="77">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C10" s="78">
         <v>28.1</v>
@@ -1704,7 +1704,7 @@
         <v>57</v>
       </c>
       <c r="B11" s="77">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C11" s="78">
         <v>0.55000000000000004</v>
@@ -1741,7 +1741,7 @@
         <v>58</v>
       </c>
       <c r="B12" s="90">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C12" s="91">
         <v>128</v>
@@ -1779,15 +1779,15 @@
       </c>
       <c r="B13" s="17">
         <f>SUM(B4:B12)</f>
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C13" s="45">
         <f>B4*C4+B5*C5+B6*C6+B7*C7+B8*C8+B9*C9+B10*C10+B11*C11+B12*C12</f>
-        <v>402.35</v>
+        <v>66.5</v>
       </c>
       <c r="D13" s="46">
         <f>B4*D4+B5*D5+B6*D6+B7*D7+B8*D8+B9*D9+B10*D10+B11*D11+D12*B12</f>
-        <v>444.89</v>
+        <v>0</v>
       </c>
       <c r="E13" s="45">
         <f>SUM(E4:E12)</f>
@@ -1795,11 +1795,11 @@
       </c>
       <c r="F13" s="45">
         <f>F12*B12+B11*F11+F10*B10+B9*F9+F8*B8+B7*F7+F6*B6+B5*F5+F4*B4</f>
-        <v>11530</v>
+        <v>1830</v>
       </c>
       <c r="G13" s="45">
         <f>G12*B12+B11*G11+G10*B10+B9*G9+G8*B8+B7*G7+G6*B6+B5*G5+G4*B4</f>
-        <v>5000</v>
+        <v>0</v>
       </c>
       <c r="H13" s="45">
         <f>SUM(H4:H12)</f>
@@ -1819,7 +1819,7 @@
       </c>
       <c r="L13" s="45">
         <f>L12*B12+B11*L11+L10*B10+B9*L9+L8*B8+B7*L7+L6*B6+B5*L5+L4*B4</f>
-        <v>2228.5714285714284</v>
+        <v>275</v>
       </c>
       <c r="M13" s="45">
         <f>SUM(M4:M12)</f>
@@ -1828,12 +1828,12 @@
       <c r="N13" s="18"/>
     </row>
     <row r="19" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="124" t="s">
+      <c r="B19" s="103" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="20" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="121" t="s">
+      <c r="B20" s="100" t="s">
         <v>67</v>
       </c>
     </row>
@@ -1877,52 +1877,52 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="31" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="96" t="s">
+      <c r="A1" s="104" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="96"/>
-      <c r="C1" s="96"/>
-      <c r="D1" s="96"/>
-      <c r="E1" s="96"/>
-      <c r="F1" s="96"/>
-      <c r="G1" s="96"/>
-      <c r="H1" s="96"/>
+      <c r="B1" s="104"/>
+      <c r="C1" s="104"/>
+      <c r="D1" s="104"/>
+      <c r="E1" s="104"/>
+      <c r="F1" s="104"/>
+      <c r="G1" s="104"/>
+      <c r="H1" s="104"/>
     </row>
     <row r="2" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="99" t="s">
+      <c r="A2" s="107" t="s">
         <v>24</v>
       </c>
-      <c r="B2" s="97" t="s">
+      <c r="B2" s="105" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="97" t="s">
+      <c r="C2" s="105" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="101" t="s">
+      <c r="D2" s="109" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="109" t="s">
+      <c r="E2" s="117" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="109" t="s">
+      <c r="F2" s="117" t="s">
         <v>14</v>
       </c>
-      <c r="G2" s="109" t="s">
+      <c r="G2" s="117" t="s">
         <v>15</v>
       </c>
-      <c r="H2" s="97" t="s">
+      <c r="H2" s="105" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="100"/>
-      <c r="B3" s="98"/>
-      <c r="C3" s="98"/>
-      <c r="D3" s="102"/>
-      <c r="E3" s="110"/>
-      <c r="F3" s="110"/>
-      <c r="G3" s="110"/>
-      <c r="H3" s="98"/>
+      <c r="A3" s="108"/>
+      <c r="B3" s="106"/>
+      <c r="C3" s="106"/>
+      <c r="D3" s="110"/>
+      <c r="E3" s="118"/>
+      <c r="F3" s="118"/>
+      <c r="G3" s="118"/>
+      <c r="H3" s="106"/>
     </row>
     <row r="4" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="72" t="s">
@@ -1949,7 +1949,7 @@
         <v>46</v>
       </c>
       <c r="B5" s="73">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C5" s="73">
         <v>11.2</v>
@@ -1984,7 +1984,7 @@
         <v>4</v>
       </c>
       <c r="C7" s="73">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="D7" s="74"/>
       <c r="E7" s="72"/>
@@ -1997,7 +1997,7 @@
         <v>25</v>
       </c>
       <c r="B8" s="20">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="C8" s="20">
         <v>453.59</v>
@@ -2016,14 +2016,14 @@
       </c>
       <c r="B9" s="24">
         <f>SUM(B4:B8)</f>
-        <v>15</v>
+        <v>10.5</v>
       </c>
       <c r="C9" s="48">
         <f>C8*B8+B7*C7+C5*B5+B4*C4+C6*B6</f>
-        <v>1431.8899999999999</v>
+        <v>1638.6849999999999</v>
       </c>
       <c r="D9" s="49">
-        <f t="shared" ref="C9:D9" si="0">SUM(D4:D8)</f>
+        <f>SUM(D4:D8)</f>
         <v>126.3</v>
       </c>
       <c r="E9" s="25"/>
@@ -2054,8 +2054,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P14"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="L16" sqref="L16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N4" sqref="N4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2066,46 +2066,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="99" t="s">
+      <c r="A1" s="107" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="97" t="s">
+      <c r="B1" s="105" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="97" t="s">
+      <c r="C1" s="105" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="101" t="s">
+      <c r="D1" s="109" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="111" t="s">
+      <c r="E1" s="119" t="s">
         <v>27</v>
       </c>
-      <c r="F1" s="113"/>
-      <c r="G1" s="111" t="s">
+      <c r="F1" s="121"/>
+      <c r="G1" s="119" t="s">
         <v>10</v>
       </c>
-      <c r="H1" s="112"/>
-      <c r="I1" s="113"/>
-      <c r="J1" s="111" t="s">
+      <c r="H1" s="120"/>
+      <c r="I1" s="121"/>
+      <c r="J1" s="119" t="s">
         <v>11</v>
       </c>
-      <c r="K1" s="112"/>
-      <c r="L1" s="113"/>
-      <c r="M1" s="111" t="s">
+      <c r="K1" s="120"/>
+      <c r="L1" s="121"/>
+      <c r="M1" s="119" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="112"/>
-      <c r="O1" s="113"/>
-      <c r="P1" s="97" t="s">
+      <c r="N1" s="120"/>
+      <c r="O1" s="121"/>
+      <c r="P1" s="105" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="100"/>
-      <c r="B2" s="98"/>
-      <c r="C2" s="98"/>
-      <c r="D2" s="102"/>
+      <c r="A2" s="108"/>
+      <c r="B2" s="106"/>
+      <c r="C2" s="106"/>
+      <c r="D2" s="110"/>
       <c r="E2" s="26" t="s">
         <v>28</v>
       </c>
@@ -2139,7 +2139,7 @@
       <c r="O2" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="P2" s="98"/>
+      <c r="P2" s="106"/>
     </row>
     <row r="3" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="66" t="s">
@@ -2170,8 +2170,8 @@
       </c>
       <c r="M3" s="69"/>
       <c r="N3" s="70">
-        <f>((9.81*TOTAL!C8/1000)^(3/2))/(4*0.11938*BattVolt*SQRT(2*PI()*1.225))/0.85</f>
-        <v>6.7050730831785783</v>
+        <f>((9.81*TOTAL!C8/1000)^(3/2))/(4*0.11938*BattVolt*SQRT(2*PI()*0.98))/0.85</f>
+        <v>6.8913217245894485</v>
       </c>
       <c r="O3" s="71">
         <v>15000</v>
@@ -2209,7 +2209,7 @@
         <v>23</v>
       </c>
       <c r="B5" s="29">
-        <f t="shared" ref="B5:O5" si="0">SUM(B3:B4)</f>
+        <f t="shared" ref="B5:M5" si="0">SUM(B3:B4)</f>
         <v>4</v>
       </c>
       <c r="C5" s="47">
@@ -2258,7 +2258,7 @@
       </c>
       <c r="N5" s="47">
         <f>4*N3*1000</f>
-        <v>26820.292332714314</v>
+        <v>27565.286898357794</v>
       </c>
       <c r="O5" s="47">
         <f>4*O3</f>
@@ -2313,10 +2313,6 @@
     <row r="14" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E14" t="s">
         <v>56</v>
-      </c>
-      <c r="H14">
-        <f>9.4/2</f>
-        <v>4.7</v>
       </c>
     </row>
   </sheetData>
@@ -2339,8 +2335,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:M9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2351,22 +2347,22 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="99"/>
-      <c r="B2" s="97" t="s">
+      <c r="A2" s="107"/>
+      <c r="B2" s="105" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="97" t="s">
+      <c r="C2" s="105" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="101" t="s">
+      <c r="D2" s="109" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="100"/>
-      <c r="B3" s="98"/>
-      <c r="C3" s="98"/>
-      <c r="D3" s="102"/>
+      <c r="A3" s="108"/>
+      <c r="B3" s="106"/>
+      <c r="C3" s="106"/>
+      <c r="D3" s="110"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
@@ -2374,15 +2370,15 @@
       </c>
       <c r="B4" s="2">
         <f>ElecQty</f>
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C4" s="2">
         <f>ElecMass</f>
-        <v>402.35</v>
+        <v>66.5</v>
       </c>
       <c r="D4" s="3">
         <f>ElecMass</f>
-        <v>402.35</v>
+        <v>66.5</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
@@ -2408,41 +2404,41 @@
       </c>
       <c r="B6" s="8">
         <f>DeadMassQty</f>
-        <v>15</v>
+        <v>10.5</v>
       </c>
       <c r="C6" s="8">
         <f>DeadMass</f>
-        <v>1431.8899999999999</v>
+        <v>1638.6849999999999</v>
       </c>
       <c r="D6" s="9">
         <f>PropMass</f>
         <v>48</v>
       </c>
-      <c r="E6" s="114" t="s">
+      <c r="E6" s="122" t="s">
         <v>59</v>
       </c>
-      <c r="F6" s="115" t="s">
+      <c r="F6" s="123" t="s">
         <v>60</v>
       </c>
-      <c r="G6" s="114" t="s">
+      <c r="G6" s="122" t="s">
         <v>61</v>
       </c>
-      <c r="H6" s="115" t="s">
+      <c r="H6" s="123" t="s">
         <v>62</v>
       </c>
-      <c r="I6" s="114" t="s">
+      <c r="I6" s="122" t="s">
         <v>39</v>
       </c>
-      <c r="J6" s="114" t="s">
+      <c r="J6" s="122" t="s">
         <v>63</v>
       </c>
-      <c r="K6" s="114" t="s">
+      <c r="K6" s="122" t="s">
         <v>64</v>
       </c>
-      <c r="L6" s="114" t="s">
+      <c r="L6" s="122" t="s">
         <v>65</v>
       </c>
-      <c r="M6" s="114" t="s">
+      <c r="M6" s="122" t="s">
         <v>38</v>
       </c>
     </row>
@@ -2462,15 +2458,15 @@
         <f>BattCostTot</f>
         <v>0</v>
       </c>
-      <c r="E7" s="114"/>
-      <c r="F7" s="116"/>
-      <c r="G7" s="114"/>
-      <c r="H7" s="116"/>
-      <c r="I7" s="114"/>
-      <c r="J7" s="114"/>
-      <c r="K7" s="114"/>
-      <c r="L7" s="114"/>
-      <c r="M7" s="114"/>
+      <c r="E7" s="122"/>
+      <c r="F7" s="124"/>
+      <c r="G7" s="122"/>
+      <c r="H7" s="124"/>
+      <c r="I7" s="122"/>
+      <c r="J7" s="122"/>
+      <c r="K7" s="122"/>
+      <c r="L7" s="122"/>
+      <c r="M7" s="122"/>
     </row>
     <row r="8" spans="1:13" s="85" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="83" t="s">
@@ -2478,61 +2474,65 @@
       </c>
       <c r="B8" s="83">
         <f>B4+B5+B6+B7</f>
-        <v>27</v>
+        <v>17.5</v>
       </c>
       <c r="C8" s="83">
         <f>C4+C5+C6+C7</f>
-        <v>2364.9399999999996</v>
+        <v>2235.8849999999998</v>
       </c>
       <c r="D8" s="84">
-        <f t="shared" ref="C8:D8" si="0">D4+D5+D6+D7</f>
-        <v>450.35</v>
-      </c>
-      <c r="E8" s="122">
+        <f t="shared" ref="D8" si="0">D4+D5+D6+D7</f>
+        <v>114.5</v>
+      </c>
+      <c r="E8" s="101">
         <f>PropThrustNom</f>
         <v>1200</v>
       </c>
-      <c r="F8" s="122">
+      <c r="F8" s="101">
         <f>PropThrustMax</f>
         <v>2400</v>
       </c>
-      <c r="G8" s="122">
+      <c r="G8" s="101">
         <f>2*C8</f>
-        <v>4729.8799999999992</v>
-      </c>
-      <c r="H8" s="122">
+        <v>4471.7699999999995</v>
+      </c>
+      <c r="H8" s="101">
         <f>BattCap</f>
         <v>4500</v>
       </c>
-      <c r="I8" s="122">
+      <c r="I8" s="101">
         <f>ElecTypPow+PropTypPow</f>
-        <v>11530</v>
-      </c>
-      <c r="J8" s="123">
+        <v>1830</v>
+      </c>
+      <c r="J8" s="102">
         <f>ElecTypCur+PropMaxCur</f>
-        <v>62228.571428571428</v>
-      </c>
-      <c r="K8" s="123">
+        <v>60275</v>
+      </c>
+      <c r="K8" s="102">
         <f>ElecTypCur+PropTypCur</f>
-        <v>29048.863761285742</v>
-      </c>
-      <c r="L8" s="122">
+        <v>27840.286898357794</v>
+      </c>
+      <c r="L8" s="101">
         <f>(H8/1000)/((K8/1000))*60</f>
-        <v>9.294683682596796</v>
-      </c>
-      <c r="M8" s="122">
+        <v>9.698175919872666</v>
+      </c>
+      <c r="M8" s="101">
         <f>(H8/1000)/(J8/1000)*60</f>
-        <v>4.3388429752066111</v>
+        <v>4.4794690999585232</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="G9">
         <f>G8/4</f>
-        <v>1182.4699999999998</v>
+        <v>1117.9424999999999</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
     <mergeCell ref="M6:M7"/>
     <mergeCell ref="E6:E7"/>
     <mergeCell ref="G6:G7"/>
@@ -2542,10 +2542,6 @@
     <mergeCell ref="F6:F7"/>
     <mergeCell ref="H6:H7"/>
     <mergeCell ref="J6:J7"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:D3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>